<commit_message>
matrix with tuple return
</commit_message>
<xml_diff>
--- a/ExcelProcesser.Tests/resources/matrixTest.xlsx
+++ b/ExcelProcesser.Tests/resources/matrixTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>一：货号，颜色，数量，配码</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>gogo</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1459,7 @@
   <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1513,6 +1519,12 @@
       </c>
       <c r="B5" t="s">
         <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11">

</xml_diff>

<commit_message>
added mxManySkipSpace and mxManyRowSkipSpace
</commit_message>
<xml_diff>
--- a/ExcelProcesser.Tests/resources/matrixTest.xlsx
+++ b/ExcelProcesser.Tests/resources/matrixTest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>一：货号，颜色，数量，配码</t>
   </si>
@@ -1462,10 +1462,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L144"/>
+  <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1476,7 +1476,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36.6">
+    <row r="1" spans="1:13" ht="36.6">
       <c r="A1" s="87"/>
       <c r="B1" s="87"/>
       <c r="C1" s="87"/>
@@ -1489,7 +1489,7 @@
       <c r="J1" s="87"/>
       <c r="K1" s="87"/>
     </row>
-    <row r="2" spans="1:11" ht="28.2">
+    <row r="2" spans="1:13" ht="28.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="88"/>
@@ -1501,7 +1501,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="28.2">
+    <row r="3" spans="1:13" ht="28.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1513,13 +1513,13 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.6" customHeight="1">
+    <row r="4" spans="1:13" ht="15.6" customHeight="1">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1533,12 +1533,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1554,8 +1557,11 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1602,12 +1608,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1617,8 +1626,17 @@
       <c r="F14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1629,7 +1647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:12">
@@ -1651,6 +1669,15 @@
       </c>
       <c r="F19" t="s">
         <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:12">

</xml_diff>